<commit_message>
Added activities comparison table
</commit_message>
<xml_diff>
--- a/040 Results/020 ESM results/Time use comparison/uktus2000.xlsx
+++ b/040 Results/020 ESM results/Time use comparison/uktus2000.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21105"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="0" windowWidth="22620" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="11940" yWindow="0" windowWidth="20860" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -750,9 +750,6 @@
     <t>Waking minutes</t>
   </si>
   <si>
-    <t>Work, study</t>
-  </si>
-  <si>
     <t>Watching TV, film</t>
   </si>
   <si>
@@ -841,18 +838,20 @@
   </si>
   <si>
     <t>Hunting, fishing</t>
+  </si>
+  <si>
+    <t>Working, studying</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -914,6 +913,22 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -941,10 +956,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1032,15 +1054,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1371,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1392,7 +1421,7 @@
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -1463,15 +1492,15 @@
         <v>642</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="G9" s="36">
         <f>D23+D26+D29+D31+D35</f>
         <v>188</v>
       </c>
       <c r="H9" s="38">
-        <f>G9/$C$4</f>
-        <v>0.20150053590568059</v>
+        <f>G9/$C$4*100</f>
+        <v>20.15005359056806</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1484,15 +1513,15 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G10" s="37">
         <f>D199+D200+D137</f>
         <v>149</v>
       </c>
       <c r="H10" s="38">
-        <f t="shared" ref="H10:H35" si="0">G10/$C$4</f>
-        <v>0.15969989281886388</v>
+        <f t="shared" ref="H10:H35" si="0">G10/$C$4*100</f>
+        <v>15.969989281886388</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1505,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G11" s="37">
         <f>D128</f>
@@ -1513,10 +1542,10 @@
       </c>
       <c r="H11" s="38">
         <f t="shared" si="0"/>
-        <v>6.1093247588424437E-2</v>
+        <v>6.109324758842444</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1529,7 +1558,7 @@
         <v>508</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G12" s="37">
         <f>D16</f>
@@ -1537,7 +1566,7 @@
       </c>
       <c r="H12" s="38">
         <f t="shared" si="0"/>
-        <v>9.3247588424437297E-2</v>
+        <v>9.32475884244373</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1550,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G13" s="37">
         <f>D205</f>
@@ -1558,7 +1587,7 @@
       </c>
       <c r="H13" s="38">
         <f t="shared" si="0"/>
-        <v>9.1103965702036438E-2</v>
+        <v>9.110396570203644</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1571,7 +1600,7 @@
         <v>507</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G14" s="35">
         <f>D46+D52+D55+D63+D76+D89</f>
@@ -1579,7 +1608,7 @@
       </c>
       <c r="H14" s="38">
         <f t="shared" si="0"/>
-        <v>8.3601286173633438E-2</v>
+        <v>8.360128617363344</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1592,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G15" s="35">
         <f>D92+D117+D217</f>
@@ -1600,7 +1629,7 @@
       </c>
       <c r="H15" s="38">
         <f t="shared" si="0"/>
-        <v>2.7867095391211148E-2</v>
+        <v>2.786709539121115</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1615,7 +1644,7 @@
         <v>87</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G16" s="35">
         <f>D49+D50+D51+D53+D54</f>
@@ -1623,7 +1652,7 @@
       </c>
       <c r="H16" s="38">
         <f t="shared" si="0"/>
-        <v>4.6087888531618437E-2</v>
+        <v>4.6087888531618439</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1636,7 +1665,7 @@
         <v>87</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G17" s="35">
         <f>D187</f>
@@ -1644,7 +1673,7 @@
       </c>
       <c r="H17" s="38">
         <f t="shared" si="0"/>
-        <v>3.2154340836012861E-3</v>
+        <v>0.32154340836012862</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1657,7 +1686,7 @@
         <v>47</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G18" s="35">
         <f>D18</f>
@@ -1665,7 +1694,7 @@
       </c>
       <c r="H18" s="38">
         <f t="shared" si="0"/>
-        <v>5.0375133976420149E-2</v>
+        <v>5.037513397642015</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1678,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G19" s="35">
         <f>D83</f>
@@ -1686,7 +1715,7 @@
       </c>
       <c r="H19" s="38">
         <f t="shared" si="0"/>
-        <v>3.3226152197213289E-2</v>
+        <v>3.322615219721329</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1699,7 +1728,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G20" s="35">
         <f>D193</f>
@@ -1707,7 +1736,7 @@
       </c>
       <c r="H20" s="38">
         <f t="shared" si="0"/>
-        <v>3.0010718113612004E-2</v>
+        <v>3.0010718113612005</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1720,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G21" s="35">
         <f>D72+D73+D74</f>
@@ -1728,7 +1757,7 @@
       </c>
       <c r="H21" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-2</v>
+        <v>1.0718113612004287</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1741,7 +1770,7 @@
         <v>175</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G22" s="35">
         <f>D15</f>
@@ -1749,7 +1778,7 @@
       </c>
       <c r="H22" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1762,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G23" s="35">
         <f>D150</f>
@@ -1770,10 +1799,10 @@
       </c>
       <c r="H23" s="38">
         <f t="shared" si="0"/>
-        <v>4.2872454448017148E-3</v>
+        <v>0.4287245444801715</v>
       </c>
       <c r="I23" s="34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1786,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G24" s="35">
         <f>D149+D151+D152+D153+D154+D155+D156+D157+D163+D146</f>
@@ -1794,7 +1823,7 @@
       </c>
       <c r="H24" s="38">
         <f t="shared" si="0"/>
-        <v>1.1789924973204717E-2</v>
+        <v>1.1789924973204717</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1807,7 +1836,7 @@
         <v>171</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G25" s="35">
         <f>D182+D175+D176</f>
@@ -1815,7 +1844,7 @@
       </c>
       <c r="H25" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1828,7 +1857,7 @@
         <v>169</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G26" s="35">
         <f>D141</f>
@@ -1836,7 +1865,7 @@
       </c>
       <c r="H26" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1849,15 +1878,15 @@
         <v>2</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G27" s="35">
-        <f>D99+D109</f>
-        <v>11</v>
+        <f>D99+D110+D111+D112+D113+D114+D115+D116+D118+D119</f>
+        <v>6</v>
       </c>
       <c r="H27" s="38">
         <f t="shared" si="0"/>
-        <v>1.1789924973204717E-2</v>
+        <v>0.64308681672025725</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1870,15 +1899,15 @@
         <v>1</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G28" s="35">
-        <f>D168</f>
+        <f>D170+D171</f>
         <v>2</v>
       </c>
       <c r="H28" s="38">
         <f t="shared" si="0"/>
-        <v>2.1436227224008574E-3</v>
+        <v>0.21436227224008575</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1891,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G29" s="35">
         <f>D184+D185+D186+D189</f>
@@ -1899,7 +1928,7 @@
       </c>
       <c r="H29" s="38">
         <f t="shared" si="0"/>
-        <v>5.3590568060021436E-3</v>
+        <v>0.53590568060021437</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1912,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G30" s="35">
         <f>D138</f>
@@ -1920,7 +1949,7 @@
       </c>
       <c r="H30" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1933,7 +1962,7 @@
         <v>3</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G31" s="35">
         <f>D123</f>
@@ -1941,10 +1970,10 @@
       </c>
       <c r="H31" s="38">
         <f t="shared" si="0"/>
-        <v>4.2872454448017148E-3</v>
+        <v>0.4287245444801715</v>
       </c>
       <c r="I31" s="34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1957,15 +1986,15 @@
         <v>0</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G32" s="35">
         <f>D71</f>
         <v>9</v>
       </c>
       <c r="H32" s="38">
-        <f>G32/$C$4</f>
-        <v>9.6463022508038593E-3</v>
+        <f t="shared" si="0"/>
+        <v>0.96463022508038598</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1978,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G33" s="35">
         <f>D139+D140</f>
@@ -1986,7 +2015,7 @@
       </c>
       <c r="H33" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1999,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G34" s="35">
         <f>D188</f>
@@ -2007,7 +2036,7 @@
       </c>
       <c r="H34" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2020,7 +2049,7 @@
         <v>15</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G35" s="35">
         <f>D160</f>
@@ -2028,7 +2057,7 @@
       </c>
       <c r="H35" s="38">
         <f t="shared" si="0"/>
-        <v>1.0718113612004287E-3</v>
+        <v>0.10718113612004287</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -4155,6 +4184,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>